<commit_message>
updated to reflect new, removed, and updated variables in final dataset
</commit_message>
<xml_diff>
--- a/output/data_dictionary_ISCO_recoded_essential_plus_health_workers.xlsx
+++ b/output/data_dictionary_ISCO_recoded_essential_plus_health_workers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\GitHub\Professions_classifications\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F59C7CF-E7B1-49D9-900A-534F992391C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE787A6-803F-482F-AFA0-BB575FF73652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B99B7C0F-8A2A-4D53-B701-B0148BA20E8E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
   <si>
     <t>Variable</t>
   </si>
@@ -107,9 +107,6 @@
     <t>job_sector.st_23</t>
   </si>
   <si>
-    <t>Hug_Date_Derniere_Soumission_C.WORK</t>
-  </si>
-  <si>
     <t>serocov_work.inc</t>
   </si>
   <si>
@@ -134,12 +131,6 @@
     <t>telework</t>
   </si>
   <si>
-    <t>physicalb</t>
-  </si>
-  <si>
-    <t>occupation</t>
-  </si>
-  <si>
     <t>occupational_grouping</t>
   </si>
   <si>
@@ -200,9 +191,6 @@
     <t>drop-down selection of job sector in the Sante-Travail 2023 questionnaire</t>
   </si>
   <si>
-    <t>For those who participated in the Sero-Cov-WORK questionnaire, the date of their most recent questionnaire submission</t>
-  </si>
-  <si>
     <t>Did the participant participate in the Sero-Cov-WORK study</t>
   </si>
   <si>
@@ -227,18 +215,9 @@
     <t>Berg, J., Ananian, S., Lieppmann, H., Mieres, F., Soares, S., Duman, A., Horne, R., Shroff, T., Sobeck, K., Song, R., &amp; International Labour Organization. Research Department. (2023). World employment and social outlook 2023: The value of essential work (1st ed.). ILO. https://doi.org/10.54394/OQVF7543</t>
   </si>
   <si>
-    <t>grouping created by Berg et al.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-digit ISCO label from the Berg et al. Paper. </t>
-  </si>
-  <si>
     <t>definition from Berg et al. --&gt; as this uses only the 2-digit codes, it's not super specific, so we might want to make our own classifications using a similar logic</t>
   </si>
   <si>
-    <t>definition from Berg et al. --&gt; as this uses only the 2-digit codes, I think this misses several occupation groups, so we probably will want to create our own list of occupation groups (based on a 3-digit code) to classify as healthcare workers</t>
-  </si>
-  <si>
     <t>binary value for teleworkability from Sostero et al. (1 = teleworkable, 0 = non-teleworkable)</t>
   </si>
   <si>
@@ -251,9 +230,6 @@
     <t>Sostero et al. 2020</t>
   </si>
   <si>
-    <t xml:space="preserve">index of physical activity (not used) from Sostero et al. </t>
-  </si>
-  <si>
     <t>Variable taken from the WORK questionnaire but I think it's not useful as it has a lot of NA and some seem to be wrong</t>
   </si>
   <si>
@@ -261,16 +237,54 @@
   </si>
   <si>
     <t>Stringhini, Silvia, María-Eugenia Zaballa, Nick Pullen, Carlos de Mestral, Javier Perez-Saez, Roxane Dumont, Attilio Picazio, et al. « Large Variation in Anti-SARS-CoV-2 Antibody Prevalence among Essential Workers in Geneva, Switzerland ». Nature Communications 12, nᵒ 1 (2021): 3455. https://doi.org/10.1038/s41467-021-23796-4.</t>
+  </si>
+  <si>
+    <t>the date of their most recent questionnaire submission</t>
+  </si>
+  <si>
+    <t>date_inclusion</t>
+  </si>
+  <si>
+    <t>date_last_submission</t>
+  </si>
+  <si>
+    <t>beyond_inclusion</t>
+  </si>
+  <si>
+    <t>date they filled the Specchio inclusion questionnaire</t>
+  </si>
+  <si>
+    <t>did they fill any questionnaire beyond the inclusion questionnaire? TRUE / FALSE</t>
+  </si>
+  <si>
+    <t>grouping created by Berg et al. based on 2-digit ISCO-08</t>
+  </si>
+  <si>
+    <t>definition from WHO classification of "health workers" that uses the ISCO-08 4-digit codes</t>
+  </si>
+  <si>
+    <t>https://www.who.int/publications/m/item/classifying-health-workers</t>
+  </si>
+  <si>
+    <t>Berg at al. 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -293,19 +307,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -316,6 +343,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{20D137B9-F405-4E0F-B839-836A1BDF4102}" name="Tableau2" displayName="Tableau2" ref="A1:C36" totalsRowShown="0">
+  <autoFilter ref="A1:C36" xr:uid="{20D137B9-F405-4E0F-B839-836A1BDF4102}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{D24AFB86-D423-4B0B-8B2D-E2EA3C9FD414}" name="Variable"/>
+    <tableColumn id="2" xr3:uid="{FCD3CF5F-823E-44D1-B2CE-2F4F7642E888}" name="Description" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{2DC580F0-C2E3-4DB3-A765-3E85C412821B}" name="Literature" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -617,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD2EE0B4-727F-452F-BBE4-2142F60CB205}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -636,7 +675,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -654,7 +693,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -662,7 +701,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -670,7 +709,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -678,7 +717,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -686,7 +725,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -694,7 +733,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="87" x14ac:dyDescent="0.35">
@@ -702,10 +741,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
@@ -713,7 +752,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -721,7 +760,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
@@ -729,7 +768,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -737,7 +776,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
@@ -745,7 +784,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -753,7 +792,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -761,7 +800,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
@@ -769,7 +808,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -777,7 +816,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -785,7 +824,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -793,7 +832,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -801,138 +840,147 @@
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
       <c r="B26" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="87" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="B31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="B32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="B33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="87" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
       <c r="B34" s="1" t="s">
-        <v>63</v>
+        <v>73</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>66</v>
+        <v>74</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C36" r:id="rId1" xr:uid="{573AE9A4-1494-49DE-A64D-381ABFA66263}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>